<commit_message>
compare result of BRISQUE
</commit_message>
<xml_diff>
--- a/images/rainfall/Compare/report.xlsx
+++ b/images/rainfall/Compare/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A__Name\parking-lot-image-processing\images\rainfall\Compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9612B626-7189-4E22-AAE2-DC540361EB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878511FD-E9C6-41E0-B410-974669302D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,10 +90,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -133,7 +133,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -146,7 +146,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>BRISQUE Score</a:t>
             </a:r>
           </a:p>
@@ -165,7 +165,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -260,7 +260,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -403,7 +403,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1383,7 +1383,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1396,14 +1396,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1426,16 +1426,16 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>17.562799999999999</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>17.1738</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>26.714400000000001</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>21.005199999999999</v>
       </c>
     </row>

</xml_diff>